<commit_message>
Add Gen CF DFT graphs
</commit_message>
<xml_diff>
--- a/data/gcf-data.xlsx
+++ b/data/gcf-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmaff/Documents/GitHub/bnl-hsrp-2020/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB675B2-E384-194A-8A2F-2F14D2C380C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12777488-104F-D24E-8FD0-20B704C5FE12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="34080" windowHeight="20280" xr2:uid="{F470DCD6-6459-9244-964D-27B17B94E1FC}"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="20280" xr2:uid="{F470DCD6-6459-9244-964D-27B17B94E1FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -234,10 +234,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$95</c:f>
+              <c:f>Sheet1!$D$2:$D$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="94"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>-13</c:v>
                 </c:pt>
@@ -649,10 +649,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$95</c:f>
+              <c:f>Sheet1!$E$2:$E$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="94"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>13</c:v>
                 </c:pt>
@@ -1064,10 +1064,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$95</c:f>
+              <c:f>Sheet1!$B$2:$B$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="94"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>13</c:v>
                 </c:pt>
@@ -1479,10 +1479,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$95</c:f>
+              <c:f>Sheet1!$C$2:$C$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="94"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>13</c:v>
                 </c:pt>
@@ -1894,10 +1894,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$95</c:f>
+              <c:f>Sheet1!$F$2:$F$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="94"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>-13</c:v>
                 </c:pt>
@@ -2309,10 +2309,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$95</c:f>
+              <c:f>Sheet1!$G$2:$G$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="94"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>13</c:v>
                 </c:pt>
@@ -2724,10 +2724,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$95</c:f>
+              <c:f>Sheet1!$H$2:$H$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="94"/>
+                <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>-1</c:v>
                 </c:pt>
@@ -7509,8 +7509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29AAFEE5-6142-AC47-A322-DDDD21DD3DCB}">
   <dimension ref="A1:W115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O80" sqref="O80"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9409,6 +9409,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>